<commit_message>
re-schedule the MBs for CAN_IDs. J1939 IDs was re-scheduled at MB16~32(for receive) and MB32~64(for transmit)
</commit_message>
<xml_diff>
--- a/LLD/Communications/MB list.xlsx
+++ b/LLD/Communications/MB list.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="97">
   <si>
     <t>Message Buffer</t>
   </si>
@@ -265,58 +265,46 @@
     <t>XTD</t>
   </si>
   <si>
-    <t>0x000000</t>
-  </si>
-  <si>
-    <t>0x00E000</t>
-  </si>
-  <si>
-    <t>0x00FEF1</t>
-  </si>
-  <si>
-    <t>0x00FDCB</t>
-  </si>
-  <si>
-    <t>0x00F004</t>
-  </si>
-  <si>
-    <t>0x00F003</t>
-  </si>
-  <si>
-    <t>0x00FDE5</t>
-  </si>
-  <si>
-    <t>0x00FEF2</t>
-  </si>
-  <si>
-    <t>0x00FEEE</t>
-  </si>
-  <si>
-    <t>0x00FEEF</t>
-  </si>
-  <si>
-    <t>0x00FEF6</t>
-  </si>
-  <si>
-    <t>0x00FEF7</t>
-  </si>
-  <si>
-    <t>0x00FEBD</t>
-  </si>
-  <si>
-    <t>0x00FEE5</t>
-  </si>
-  <si>
-    <t>0x00FDC5</t>
-  </si>
-  <si>
-    <t>0x00EA00</t>
-  </si>
-  <si>
-    <t>0x00FECA</t>
-  </si>
-  <si>
-    <t>0x00DF00</t>
+    <t>0x18EA0000</t>
+  </si>
+  <si>
+    <t>0x18EB0000</t>
+  </si>
+  <si>
+    <t>0x18EC0000</t>
+  </si>
+  <si>
+    <t>0x18FEF7D5</t>
+  </si>
+  <si>
+    <t>0x18FEF8D5</t>
+  </si>
+  <si>
+    <t>0x18FEF9D5</t>
+  </si>
+  <si>
+    <t>0x18FEFAD5</t>
+  </si>
+  <si>
+    <t>0x18FEFBD5</t>
+  </si>
+  <si>
+    <t>0x18FEFCD0</t>
+  </si>
+  <si>
+    <t>0x18FEFDD0</t>
+  </si>
+  <si>
+    <t>0x18FEFED0</t>
+  </si>
+  <si>
+    <t>0x18FEFFD0</t>
+  </si>
+  <si>
+    <t>0x08FF10D5</t>
+  </si>
+  <si>
+    <t>0x1FFFFFFF</t>
   </si>
 </sst>
 </file>
@@ -661,14 +649,14 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J46" sqref="J46"/>
+      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -765,26 +753,101 @@
       <c r="A10" t="s">
         <v>13</v>
       </c>
+      <c r="B10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
+      <c r="B11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
+      <c r="B12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
+      <c r="B13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
+      <c r="B14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -795,11 +858,41 @@
       <c r="A16" t="s">
         <v>19</v>
       </c>
+      <c r="B16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
+      <c r="B17" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -809,16 +902,16 @@
         <v>74</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="F18" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -829,16 +922,16 @@
         <v>74</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>75</v>
+      <c r="F19" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -849,16 +942,16 @@
         <v>74</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="E20">
         <v>0</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>76</v>
+      <c r="F20" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -869,16 +962,16 @@
         <v>74</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="E21">
         <v>0</v>
       </c>
       <c r="F21" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -889,51 +982,96 @@
         <v>74</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="E22">
         <v>0</v>
       </c>
       <c r="F22" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>26</v>
       </c>
+      <c r="B23" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>82</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>27</v>
       </c>
+      <c r="B24" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>82</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>28</v>
       </c>
+      <c r="B25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>82</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="E26">
         <v>0</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>81</v>
+      <c r="F26" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -941,35 +1079,80 @@
         <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="E27">
         <v>0</v>
       </c>
-      <c r="F27" s="2" t="s">
-        <v>80</v>
+      <c r="F27" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>31</v>
       </c>
+      <c r="B28" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>82</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>32</v>
       </c>
+      <c r="B29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>33</v>
       </c>
+      <c r="B30" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>82</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -991,7 +1174,7 @@
         <v>37</v>
       </c>
       <c r="B34" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -1003,7 +1186,7 @@
         <v>0</v>
       </c>
       <c r="F34" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1011,7 +1194,7 @@
         <v>38</v>
       </c>
       <c r="B35" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -1023,48 +1206,18 @@
         <v>0</v>
       </c>
       <c r="F35" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>39</v>
       </c>
-      <c r="B36" t="s">
-        <v>74</v>
-      </c>
-      <c r="C36">
-        <v>1</v>
-      </c>
-      <c r="D36" t="s">
-        <v>82</v>
-      </c>
-      <c r="E36">
-        <v>0</v>
-      </c>
-      <c r="F36" t="s">
-        <v>85</v>
-      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>40</v>
       </c>
-      <c r="B37" t="s">
-        <v>74</v>
-      </c>
-      <c r="C37">
-        <v>1</v>
-      </c>
-      <c r="D37" t="s">
-        <v>82</v>
-      </c>
-      <c r="E37">
-        <v>0</v>
-      </c>
-      <c r="F37" t="s">
-        <v>86</v>
-      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -1121,292 +1274,82 @@
         <v>51</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>53</v>
       </c>
-      <c r="B50" t="s">
-        <v>79</v>
-      </c>
-      <c r="C50">
-        <v>1</v>
-      </c>
-      <c r="D50" t="s">
-        <v>82</v>
-      </c>
-      <c r="E50">
-        <v>0</v>
-      </c>
-      <c r="F50" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>54</v>
       </c>
-      <c r="B51" t="s">
-        <v>79</v>
-      </c>
-      <c r="C51">
-        <v>1</v>
-      </c>
-      <c r="D51" t="s">
-        <v>82</v>
-      </c>
-      <c r="E51">
-        <v>0</v>
-      </c>
-      <c r="F51" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>55</v>
       </c>
-      <c r="B52" t="s">
-        <v>79</v>
-      </c>
-      <c r="C52">
-        <v>1</v>
-      </c>
-      <c r="D52" t="s">
-        <v>82</v>
-      </c>
-      <c r="E52">
-        <v>0</v>
-      </c>
-      <c r="F52" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>56</v>
       </c>
-      <c r="B53" t="s">
-        <v>79</v>
-      </c>
-      <c r="C53">
-        <v>1</v>
-      </c>
-      <c r="D53" t="s">
-        <v>82</v>
-      </c>
-      <c r="E53">
-        <v>0</v>
-      </c>
-      <c r="F53" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>57</v>
       </c>
-      <c r="B54" t="s">
-        <v>79</v>
-      </c>
-      <c r="C54">
-        <v>1</v>
-      </c>
-      <c r="D54" t="s">
-        <v>82</v>
-      </c>
-      <c r="E54">
-        <v>0</v>
-      </c>
-      <c r="F54" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>58</v>
       </c>
-      <c r="B55" t="s">
-        <v>79</v>
-      </c>
-      <c r="C55">
-        <v>1</v>
-      </c>
-      <c r="D55" t="s">
-        <v>82</v>
-      </c>
-      <c r="E55">
-        <v>0</v>
-      </c>
-      <c r="F55" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>59</v>
       </c>
-      <c r="B56" t="s">
-        <v>79</v>
-      </c>
-      <c r="C56">
-        <v>1</v>
-      </c>
-      <c r="D56" t="s">
-        <v>82</v>
-      </c>
-      <c r="E56">
-        <v>0</v>
-      </c>
-      <c r="F56" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>60</v>
       </c>
-      <c r="B57" t="s">
-        <v>79</v>
-      </c>
-      <c r="C57">
-        <v>1</v>
-      </c>
-      <c r="D57" t="s">
-        <v>82</v>
-      </c>
-      <c r="E57">
-        <v>0</v>
-      </c>
-      <c r="F57" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>61</v>
       </c>
-      <c r="B58" t="s">
-        <v>79</v>
-      </c>
-      <c r="C58">
-        <v>1</v>
-      </c>
-      <c r="D58" t="s">
-        <v>82</v>
-      </c>
-      <c r="E58">
-        <v>0</v>
-      </c>
-      <c r="F58" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>62</v>
       </c>
-      <c r="B59" t="s">
-        <v>79</v>
-      </c>
-      <c r="C59">
-        <v>1</v>
-      </c>
-      <c r="D59" t="s">
-        <v>82</v>
-      </c>
-      <c r="E59">
-        <v>0</v>
-      </c>
-      <c r="F59" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>63</v>
       </c>
-      <c r="B60" t="s">
-        <v>79</v>
-      </c>
-      <c r="C60">
-        <v>1</v>
-      </c>
-      <c r="D60" t="s">
-        <v>82</v>
-      </c>
-      <c r="E60">
-        <v>0</v>
-      </c>
-      <c r="F60" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>64</v>
       </c>
-      <c r="B61" t="s">
-        <v>79</v>
-      </c>
-      <c r="C61">
-        <v>1</v>
-      </c>
-      <c r="D61" t="s">
-        <v>82</v>
-      </c>
-      <c r="E61">
-        <v>0</v>
-      </c>
-      <c r="F61" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>65</v>
       </c>
-      <c r="B62" t="s">
-        <v>79</v>
-      </c>
-      <c r="C62">
-        <v>1</v>
-      </c>
-      <c r="D62" t="s">
-        <v>82</v>
-      </c>
-      <c r="E62">
-        <v>0</v>
-      </c>
-      <c r="F62" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>66</v>
       </c>
-      <c r="B63" t="s">
-        <v>79</v>
-      </c>
-      <c r="C63">
-        <v>1</v>
-      </c>
-      <c r="D63" t="s">
-        <v>82</v>
-      </c>
-      <c r="E63">
-        <v>0</v>
-      </c>
-      <c r="F63" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>67</v>
       </c>

</xml_diff>